<commit_message>
arbol asbtracto para las pruebas correcto
</commit_message>
<xml_diff>
--- a/ConjuntosPrimeroSiguienteYTabla.xlsx
+++ b/ConjuntosPrimeroSiguienteYTabla.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,6 +19,7 @@
     <definedName name="ap">Hoja1!$F$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1425,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99923972-C091-4E9D-9C54-8623750091A9}">
   <dimension ref="A1:CJ303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E104" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L111" sqref="L111"/>
+    <sheetView tabSelected="1" topLeftCell="BW126" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CH147" sqref="CH147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21864,7 +21865,7 @@
         <v>143</v>
       </c>
       <c r="N111" s="15" t="str">
-        <f t="shared" ref="M111:AG111" si="110">IF(N264="", "", CONCATENATE("d", N264))</f>
+        <f t="shared" ref="N111:AG111" si="110">IF(N264="", "", CONCATENATE("d", N264))</f>
         <v/>
       </c>
       <c r="O111" s="15" t="s">

</xml_diff>